<commit_message>
Fixed with the new version of Kayak.com
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData-Kayak.xlsx
+++ b/src/test/resources/TestData-Kayak.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walia\eclipse-workspace\AutomationProject\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walia\git\Kayak-Automation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EDC0F1-A03D-4439-898C-BC1FD902A797}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE43439-8913-4897-9100-86C37E964D35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3C9D7627-B5BE-40C0-AE7E-29F1BE65B0A4}"/>
+    <workbookView xWindow="1428" yWindow="1428" windowWidth="17280" windowHeight="8964" xr2:uid="{3C9D7627-B5BE-40C0-AE7E-29F1BE65B0A4}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Origin</t>
   </si>
@@ -40,21 +40,6 @@
     <t>Destination</t>
   </si>
   <si>
-    <t>Oakland</t>
-  </si>
-  <si>
-    <t>Las Vegas(LAS)</t>
-  </si>
-  <si>
-    <t>San Francisco(SFO)</t>
-  </si>
-  <si>
-    <t>Atlanta(ATL)</t>
-  </si>
-  <si>
-    <t>CLT</t>
-  </si>
-  <si>
     <t>DepartureDate</t>
   </si>
   <si>
@@ -64,30 +49,6 @@
     <t>Record 1</t>
   </si>
   <si>
-    <t>Record 2</t>
-  </si>
-  <si>
-    <t>Record 3</t>
-  </si>
-  <si>
-    <t>11/20</t>
-  </si>
-  <si>
-    <t>11/25</t>
-  </si>
-  <si>
-    <t>10/12</t>
-  </si>
-  <si>
-    <t>10/19</t>
-  </si>
-  <si>
-    <t>12/1</t>
-  </si>
-  <si>
-    <t>12/15</t>
-  </si>
-  <si>
     <t>Origin Include Near By Airports</t>
   </si>
   <si>
@@ -98,6 +59,33 @@
   </si>
   <si>
     <t>FALSE</t>
+  </si>
+  <si>
+    <t>05/20/2020</t>
+  </si>
+  <si>
+    <t>05/25/2020</t>
+  </si>
+  <si>
+    <t>OAK</t>
+  </si>
+  <si>
+    <t>Las Vegas (LAS)</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>SFO</t>
+  </si>
+  <si>
+    <t>Oakland (OAK)</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -141,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -153,6 +141,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,109 +462,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46F12C5D-F831-48AB-AB16-8185425C432C}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.77734375" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="27.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="27.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" customWidth="1"/>
     <col min="6" max="6" width="14.6640625" customWidth="1"/>
     <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>18</v>
+      <c r="C1" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="G3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>